<commit_message>
add 2019 to GovExpEdu
</commit_message>
<xml_diff>
--- a/data/GovExpEdu.xlsx
+++ b/data/GovExpEdu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Bocconi\Simulation\Final\Model\SMFinal_Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7630DF13-99EE-442B-A4A4-6D96AC8FCB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{920ADD7C-FC15-4853-98D5-D747469867A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5164" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5381" uniqueCount="243">
   <si>
     <t>St. Lucia</t>
   </si>
@@ -1090,15 +1090,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AN218"/>
+  <dimension ref="A1:AO218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AO2" sqref="AO2:AO218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>168</v>
       </c>
@@ -1219,8 +1219,11 @@
       <c r="AN1">
         <v>2018</v>
       </c>
+      <c r="AO1">
+        <v>2019</v>
+      </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>183</v>
       </c>
@@ -1341,8 +1344,11 @@
       <c r="AN2">
         <v>0.48597481999999997</v>
       </c>
+      <c r="AO2" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>165</v>
       </c>
@@ -1463,8 +1469,11 @@
       <c r="AN3">
         <v>2.8415393799999999</v>
       </c>
+      <c r="AO3" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1585,8 +1594,11 @@
       <c r="AN4">
         <v>4.09385347</v>
       </c>
+      <c r="AO4" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>42</v>
       </c>
@@ -1707,8 +1719,11 @@
       <c r="AN5" t="s">
         <v>154</v>
       </c>
+      <c r="AO5" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>167</v>
       </c>
@@ -1829,8 +1844,11 @@
       <c r="AN6">
         <v>4.5586490599999996</v>
       </c>
+      <c r="AO6" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1951,8 +1969,11 @@
       <c r="AN7">
         <v>1.0687836399999999</v>
       </c>
+      <c r="AO7" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>94</v>
       </c>
@@ -2073,8 +2094,11 @@
       <c r="AN8">
         <v>2.9041159200000002</v>
       </c>
+      <c r="AO8" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -2195,8 +2219,11 @@
       <c r="AN9">
         <v>5.9101710299999999</v>
       </c>
+      <c r="AO9" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -2317,8 +2344,11 @@
       <c r="AN10">
         <v>1.23714364</v>
       </c>
+      <c r="AO10" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>223</v>
       </c>
@@ -2439,8 +2469,11 @@
       <c r="AN11" t="s">
         <v>154</v>
       </c>
+      <c r="AO11" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>193</v>
       </c>
@@ -2561,8 +2594,11 @@
       <c r="AN12">
         <v>6.4124374399999997</v>
       </c>
+      <c r="AO12" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2683,8 +2719,11 @@
       <c r="AN13">
         <v>7.5464735000000003</v>
       </c>
+      <c r="AO13" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>204</v>
       </c>
@@ -2805,8 +2844,11 @@
       <c r="AN14">
         <v>0.93211520000000003</v>
       </c>
+      <c r="AO14" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>144</v>
       </c>
@@ -2927,8 +2969,11 @@
       <c r="AN15">
         <v>3.1381137400000001</v>
       </c>
+      <c r="AO15" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>206</v>
       </c>
@@ -3049,8 +3094,11 @@
       <c r="AN16">
         <v>2.4318726100000001</v>
       </c>
+      <c r="AO16" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>180</v>
       </c>
@@ -3171,8 +3219,11 @@
       <c r="AN17">
         <v>0.39778790000000003</v>
       </c>
+      <c r="AO17" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>101</v>
       </c>
@@ -3293,8 +3344,11 @@
       <c r="AN18">
         <v>2.9384310199999999</v>
       </c>
+      <c r="AO18" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>208</v>
       </c>
@@ -3415,8 +3469,11 @@
       <c r="AN19">
         <v>3.9742019200000001</v>
       </c>
+      <c r="AO19" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>211</v>
       </c>
@@ -3537,8 +3594,11 @@
       <c r="AN20">
         <v>7.8199439000000002</v>
       </c>
+      <c r="AO20" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>218</v>
       </c>
@@ -3659,8 +3719,11 @@
       <c r="AN21">
         <v>3.90398026</v>
       </c>
+      <c r="AO21" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>115</v>
       </c>
@@ -3781,8 +3844,11 @@
       <c r="AN22">
         <v>0.49050966000000001</v>
       </c>
+      <c r="AO22" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -3903,8 +3969,11 @@
       <c r="AN23" t="s">
         <v>154</v>
       </c>
+      <c r="AO23" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>31</v>
       </c>
@@ -4025,8 +4094,11 @@
       <c r="AN24">
         <v>2.43216681</v>
       </c>
+      <c r="AO24" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>178</v>
       </c>
@@ -4147,8 +4219,11 @@
       <c r="AN25">
         <v>4.4843430499999997</v>
       </c>
+      <c r="AO25" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>169</v>
       </c>
@@ -4269,8 +4344,11 @@
       <c r="AN26">
         <v>6.2131824499999997</v>
       </c>
+      <c r="AO26" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -4391,8 +4469,11 @@
       <c r="AN27">
         <v>4.5309739100000002</v>
       </c>
+      <c r="AO27" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>207</v>
       </c>
@@ -4513,8 +4594,11 @@
       <c r="AN28">
         <v>3.9648194299999999</v>
       </c>
+      <c r="AO28" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -4635,8 +4719,11 @@
       <c r="AN29" t="s">
         <v>154</v>
       </c>
+      <c r="AO29" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>107</v>
       </c>
@@ -4757,8 +4844,11 @@
       <c r="AN30">
         <v>2.2956669299999999</v>
       </c>
+      <c r="AO30" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -4879,8 +4969,11 @@
       <c r="AN31">
         <v>4.2343692800000001</v>
       </c>
+      <c r="AO31" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>133</v>
       </c>
@@ -5001,8 +5094,11 @@
       <c r="AN32">
         <v>2.3925394999999998</v>
       </c>
+      <c r="AO32" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>234</v>
       </c>
@@ -5123,8 +5219,11 @@
       <c r="AN33">
         <v>1.90243125</v>
       </c>
+      <c r="AO33" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>108</v>
       </c>
@@ -5245,8 +5344,11 @@
       <c r="AN34">
         <v>3.2248084499999998</v>
       </c>
+      <c r="AO34" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>122</v>
       </c>
@@ -5367,8 +5469,11 @@
       <c r="AN35">
         <v>1.2820390500000001</v>
       </c>
+      <c r="AO35" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>41</v>
       </c>
@@ -5489,8 +5594,11 @@
       <c r="AN36">
         <v>0.21037169</v>
       </c>
+      <c r="AO36" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>179</v>
       </c>
@@ -5611,8 +5719,11 @@
       <c r="AN37">
         <v>7.9301104499999999</v>
       </c>
+      <c r="AO37" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>222</v>
       </c>
@@ -5733,8 +5844,11 @@
       <c r="AN38" t="s">
         <v>154</v>
       </c>
+      <c r="AO38" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -5855,8 +5969,11 @@
       <c r="AN39">
         <v>0.68838823000000005</v>
       </c>
+      <c r="AO39" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -5977,8 +6094,11 @@
       <c r="AN40">
         <v>0.69685549000000002</v>
       </c>
+      <c r="AO40" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>84</v>
       </c>
@@ -6099,8 +6219,11 @@
       <c r="AN41" t="s">
         <v>154</v>
       </c>
+      <c r="AO41" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>238</v>
       </c>
@@ -6221,8 +6344,11 @@
       <c r="AN42">
         <v>4.6468858700000002</v>
       </c>
+      <c r="AO42" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>161</v>
       </c>
@@ -6343,8 +6469,11 @@
       <c r="AN43">
         <v>3.018888</v>
       </c>
+      <c r="AO43" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>191</v>
       </c>
@@ -6465,8 +6594,11 @@
       <c r="AN44">
         <v>5.4712009400000001</v>
       </c>
+      <c r="AO44" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>225</v>
       </c>
@@ -6587,8 +6719,11 @@
       <c r="AN45">
         <v>0.42495197000000001</v>
       </c>
+      <c r="AO45" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -6709,8 +6844,11 @@
       <c r="AN46">
         <v>0.49770062999999998</v>
       </c>
+      <c r="AO46" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>72</v>
       </c>
@@ -6831,8 +6969,11 @@
       <c r="AN47">
         <v>0.78597682999999996</v>
       </c>
+      <c r="AO47" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>152</v>
       </c>
@@ -6953,8 +7094,11 @@
       <c r="AN48">
         <v>5.4754152300000003</v>
       </c>
+      <c r="AO48" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="49" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>96</v>
       </c>
@@ -7075,8 +7219,11 @@
       <c r="AN49">
         <v>1.2072671699999999</v>
       </c>
+      <c r="AO49" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="50" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>235</v>
       </c>
@@ -7197,8 +7344,11 @@
       <c r="AN50">
         <v>5.6807222399999997</v>
       </c>
+      <c r="AO50" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="51" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>77</v>
       </c>
@@ -7319,8 +7469,11 @@
       <c r="AN51">
         <v>9.9462337499999993</v>
       </c>
+      <c r="AO51" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="52" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>189</v>
       </c>
@@ -7441,8 +7594,11 @@
       <c r="AN52" t="s">
         <v>154</v>
       </c>
+      <c r="AO52" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="53" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>97</v>
       </c>
@@ -7563,8 +7719,11 @@
       <c r="AN53">
         <v>2.8975887299999998</v>
       </c>
+      <c r="AO53" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="54" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>90</v>
       </c>
@@ -7685,8 +7844,11 @@
       <c r="AN54">
         <v>6.3239545799999997</v>
       </c>
+      <c r="AO54" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="55" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>163</v>
       </c>
@@ -7807,8 +7969,11 @@
       <c r="AN55">
         <v>8.4473724400000005</v>
       </c>
+      <c r="AO55" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="56" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>104</v>
       </c>
@@ -7929,8 +8094,11 @@
       <c r="AN56">
         <v>1.15207028</v>
       </c>
+      <c r="AO56" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="57" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -8051,8 +8219,11 @@
       <c r="AN57">
         <v>4.2720928200000001</v>
       </c>
+      <c r="AO57" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="58" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -8173,8 +8344,11 @@
       <c r="AN58">
         <v>2.5401179800000002</v>
       </c>
+      <c r="AO58" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="59" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>18</v>
       </c>
@@ -8295,8 +8469,11 @@
       <c r="AN59">
         <v>4.2304620699999997</v>
       </c>
+      <c r="AO59" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="60" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>139</v>
       </c>
@@ -8417,8 +8594,11 @@
       <c r="AN60">
         <v>1.4215319200000001</v>
       </c>
+      <c r="AO60" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="61" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>148</v>
       </c>
@@ -8539,8 +8719,11 @@
       <c r="AN61">
         <v>4.53943443</v>
       </c>
+      <c r="AO61" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="62" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>29</v>
       </c>
@@ -8661,8 +8844,11 @@
       <c r="AN62">
         <v>0.59562802000000004</v>
       </c>
+      <c r="AO62" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="63" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>118</v>
       </c>
@@ -8783,8 +8969,11 @@
       <c r="AN63">
         <v>0.63723993000000001</v>
       </c>
+      <c r="AO63" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="64" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>80</v>
       </c>
@@ -8905,8 +9094,11 @@
       <c r="AN64">
         <v>4.9205517800000003</v>
       </c>
+      <c r="AO64" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="65" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>20</v>
       </c>
@@ -9027,8 +9219,11 @@
       <c r="AN65">
         <v>0.77011490000000005</v>
       </c>
+      <c r="AO65" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="66" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>213</v>
       </c>
@@ -9149,8 +9344,11 @@
       <c r="AN66" t="s">
         <v>154</v>
       </c>
+      <c r="AO66" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="67" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>47</v>
       </c>
@@ -9271,8 +9469,11 @@
       <c r="AN67">
         <v>2.3386900399999999</v>
       </c>
+      <c r="AO67" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="68" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -9393,8 +9594,11 @@
       <c r="AN68">
         <v>7.0994348499999997</v>
       </c>
+      <c r="AO68" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="69" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -9515,8 +9719,11 @@
       <c r="AN69">
         <v>8.26006222</v>
       </c>
+      <c r="AO69" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="70" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>85</v>
       </c>
@@ -9637,8 +9844,11 @@
       <c r="AN70" t="s">
         <v>154</v>
       </c>
+      <c r="AO70" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="71" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>160</v>
       </c>
@@ -9759,8 +9969,11 @@
       <c r="AN71">
         <v>1.60855591</v>
       </c>
+      <c r="AO71" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="72" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>135</v>
       </c>
@@ -9881,8 +10094,11 @@
       <c r="AN72">
         <v>0.94653189000000004</v>
       </c>
+      <c r="AO72" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="73" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>106</v>
       </c>
@@ -10003,8 +10219,11 @@
       <c r="AN73">
         <v>2.80701351</v>
       </c>
+      <c r="AO73" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="74" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>3</v>
       </c>
@@ -10125,8 +10344,11 @@
       <c r="AN74">
         <v>8.8792486200000003</v>
       </c>
+      <c r="AO74" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="75" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>140</v>
       </c>
@@ -10247,8 +10469,11 @@
       <c r="AN75">
         <v>1.37637711</v>
       </c>
+      <c r="AO75" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="76" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>63</v>
       </c>
@@ -10369,8 +10594,11 @@
       <c r="AN76" t="s">
         <v>154</v>
       </c>
+      <c r="AO76" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="77" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>173</v>
       </c>
@@ -10491,8 +10719,11 @@
       <c r="AN77">
         <v>4.0068788499999997</v>
       </c>
+      <c r="AO77" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="78" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>24</v>
       </c>
@@ -10613,8 +10844,11 @@
       <c r="AN78" t="s">
         <v>154</v>
       </c>
+      <c r="AO78" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="79" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -10735,8 +10969,11 @@
       <c r="AN79">
         <v>1.70504856</v>
       </c>
+      <c r="AO79" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="80" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>212</v>
       </c>
@@ -10857,8 +11094,11 @@
       <c r="AN80" t="s">
         <v>154</v>
       </c>
+      <c r="AO80" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="81" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>46</v>
       </c>
@@ -10979,8 +11219,11 @@
       <c r="AN81">
         <v>2.05508208</v>
       </c>
+      <c r="AO81" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="82" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>126</v>
       </c>
@@ -11101,8 +11344,11 @@
       <c r="AN82">
         <v>0.6463778</v>
       </c>
+      <c r="AO82" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="83" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>43</v>
       </c>
@@ -11223,8 +11469,11 @@
       <c r="AN83">
         <v>0.64091021000000004</v>
       </c>
+      <c r="AO83" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="84" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -11345,8 +11594,11 @@
       <c r="AN84">
         <v>3.6728050699999999</v>
       </c>
+      <c r="AO84" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="85" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>116</v>
       </c>
@@ -11467,8 +11719,11 @@
       <c r="AN85">
         <v>0.92181933000000005</v>
       </c>
+      <c r="AO85" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="86" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>150</v>
       </c>
@@ -11589,8 +11844,11 @@
       <c r="AN86">
         <v>2.8381052000000002</v>
       </c>
+      <c r="AO86" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="87" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>171</v>
       </c>
@@ -11711,8 +11969,11 @@
       <c r="AN87" t="s">
         <v>154</v>
       </c>
+      <c r="AO87" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="88" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>220</v>
       </c>
@@ -11833,8 +12094,11 @@
       <c r="AN88">
         <v>4.6297883999999998</v>
       </c>
+      <c r="AO88" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="89" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>30</v>
       </c>
@@ -11955,8 +12219,11 @@
       <c r="AN89">
         <v>6.9763226500000002</v>
       </c>
+      <c r="AO89" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="90" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>228</v>
       </c>
@@ -12077,8 +12344,11 @@
       <c r="AN90">
         <v>0.95529788999999998</v>
       </c>
+      <c r="AO90" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="91" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>137</v>
       </c>
@@ -12199,8 +12469,11 @@
       <c r="AN91">
         <v>1.4160132400000001</v>
       </c>
+      <c r="AO91" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="92" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>121</v>
       </c>
@@ -12321,8 +12594,11 @@
       <c r="AN92">
         <v>3.97810006</v>
       </c>
+      <c r="AO92" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="93" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>78</v>
       </c>
@@ -12443,8 +12719,11 @@
       <c r="AN93">
         <v>1.9763942999999999</v>
       </c>
+      <c r="AO93" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="94" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>89</v>
       </c>
@@ -12565,8 +12844,11 @@
       <c r="AN94">
         <v>5.1197037700000001</v>
       </c>
+      <c r="AO94" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="95" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>155</v>
       </c>
@@ -12687,8 +12969,11 @@
       <c r="AN95" t="s">
         <v>154</v>
       </c>
+      <c r="AO95" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="96" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -12809,8 +13094,11 @@
       <c r="AN96">
         <v>4.8638315199999997</v>
       </c>
+      <c r="AO96" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="97" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>202</v>
       </c>
@@ -12931,8 +13219,11 @@
       <c r="AN97">
         <v>6.4043731700000004</v>
       </c>
+      <c r="AO97" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="98" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>164</v>
       </c>
@@ -13053,8 +13344,11 @@
       <c r="AN98">
         <v>3.9362068200000002</v>
       </c>
+      <c r="AO98" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="99" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>100</v>
       </c>
@@ -13175,8 +13469,11 @@
       <c r="AN99">
         <v>9.2106161100000001</v>
       </c>
+      <c r="AO99" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="100" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>215</v>
       </c>
@@ -13297,8 +13594,11 @@
       <c r="AN100">
         <v>3.83110499</v>
       </c>
+      <c r="AO100" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="101" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>221</v>
       </c>
@@ -13419,8 +13719,11 @@
       <c r="AN101">
         <v>1.7777290299999999</v>
       </c>
+      <c r="AO101" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="102" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>136</v>
       </c>
@@ -13541,8 +13844,11 @@
       <c r="AN102">
         <v>2.1773498099999999</v>
       </c>
+      <c r="AO102" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="103" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>14</v>
       </c>
@@ -13663,8 +13969,11 @@
       <c r="AN103">
         <v>9.2531051600000005</v>
       </c>
+      <c r="AO103" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="104" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>194</v>
       </c>
@@ -13785,8 +14094,11 @@
       <c r="AN104" t="s">
         <v>154</v>
       </c>
+      <c r="AO104" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="105" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>73</v>
       </c>
@@ -13907,8 +14219,11 @@
       <c r="AN105">
         <v>4.4208488499999996</v>
       </c>
+      <c r="AO105" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="106" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>8</v>
       </c>
@@ -14029,8 +14344,11 @@
       <c r="AN106" t="s">
         <v>154</v>
       </c>
+      <c r="AO106" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="107" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>55</v>
       </c>
@@ -14151,8 +14469,11 @@
       <c r="AN107">
         <v>4.4014334699999997</v>
       </c>
+      <c r="AO107" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="108" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>181</v>
       </c>
@@ -14273,8 +14594,11 @@
       <c r="AN108">
         <v>2.7989799999999998</v>
       </c>
+      <c r="AO108" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="109" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>9</v>
       </c>
@@ -14395,8 +14719,11 @@
       <c r="AN109">
         <v>0.86922860000000002</v>
       </c>
+      <c r="AO109" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="110" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>62</v>
       </c>
@@ -14517,8 +14844,11 @@
       <c r="AN110">
         <v>3.69595933</v>
       </c>
+      <c r="AO110" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="111" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>16</v>
       </c>
@@ -14639,8 +14969,11 @@
       <c r="AN111">
         <v>4.1782774900000001</v>
       </c>
+      <c r="AO111" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="112" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>200</v>
       </c>
@@ -14761,8 +15094,11 @@
       <c r="AN112">
         <v>5.3902568799999999</v>
       </c>
+      <c r="AO112" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="113" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>129</v>
       </c>
@@ -14883,8 +15219,11 @@
       <c r="AN113">
         <v>1.69556665</v>
       </c>
+      <c r="AO113" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="114" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>203</v>
       </c>
@@ -15005,8 +15344,11 @@
       <c r="AN114" t="s">
         <v>154</v>
       </c>
+      <c r="AO114" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="115" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>36</v>
       </c>
@@ -15127,8 +15469,11 @@
       <c r="AN115" t="s">
         <v>154</v>
       </c>
+      <c r="AO115" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="116" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>187</v>
       </c>
@@ -15249,8 +15594,11 @@
       <c r="AN116">
         <v>4.3258891100000003</v>
       </c>
+      <c r="AO116" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="117" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>109</v>
       </c>
@@ -15371,8 +15719,11 @@
       <c r="AN117">
         <v>4.4888224599999997</v>
       </c>
+      <c r="AO117" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="118" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>7</v>
       </c>
@@ -15493,8 +15844,11 @@
       <c r="AN118" t="s">
         <v>154</v>
       </c>
+      <c r="AO118" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="119" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>112</v>
       </c>
@@ -15615,8 +15969,11 @@
       <c r="AN119">
         <v>3.7734344000000002</v>
       </c>
+      <c r="AO119" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="120" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>229</v>
       </c>
@@ -15737,8 +16094,11 @@
       <c r="AN120">
         <v>1.7113918100000001</v>
       </c>
+      <c r="AO120" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="121" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>209</v>
       </c>
@@ -15859,8 +16219,11 @@
       <c r="AN121">
         <v>2.6956946799999999</v>
       </c>
+      <c r="AO121" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="122" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>125</v>
       </c>
@@ -15981,8 +16344,11 @@
       <c r="AN122">
         <v>1.9225193300000001</v>
       </c>
+      <c r="AO122" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="123" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>146</v>
       </c>
@@ -16103,8 +16469,11 @@
       <c r="AN123">
         <v>6.6466660500000003</v>
       </c>
+      <c r="AO123" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="124" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>141</v>
       </c>
@@ -16225,8 +16594,11 @@
       <c r="AN124">
         <v>1.0963175300000001</v>
       </c>
+      <c r="AO124" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="125" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>113</v>
       </c>
@@ -16347,8 +16719,11 @@
       <c r="AN125">
         <v>5.6904973999999999</v>
       </c>
+      <c r="AO125" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="126" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>32</v>
       </c>
@@ -16469,8 +16844,11 @@
       <c r="AN126">
         <v>7.6224794400000002</v>
       </c>
+      <c r="AO126" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="127" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>147</v>
       </c>
@@ -16591,8 +16969,11 @@
       <c r="AN127">
         <v>1.64334965</v>
       </c>
+      <c r="AO127" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="128" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>226</v>
       </c>
@@ -16713,8 +17094,11 @@
       <c r="AN128">
         <v>2.51386142</v>
       </c>
+      <c r="AO128" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="129" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>227</v>
       </c>
@@ -16835,8 +17219,11 @@
       <c r="AN129">
         <v>2.6895785299999999</v>
       </c>
+      <c r="AO129" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="130" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>131</v>
       </c>
@@ -16957,8 +17344,11 @@
       <c r="AN130">
         <v>3.3142621499999998</v>
       </c>
+      <c r="AO130" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="131" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>86</v>
       </c>
@@ -17079,8 +17469,11 @@
       <c r="AN131">
         <v>3.7281441700000002</v>
       </c>
+      <c r="AO131" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="132" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>143</v>
       </c>
@@ -17201,8 +17594,11 @@
       <c r="AN132">
         <v>1.36923087</v>
       </c>
+      <c r="AO132" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="133" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>56</v>
       </c>
@@ -17323,8 +17719,11 @@
       <c r="AN133">
         <v>2.2227485200000001</v>
       </c>
+      <c r="AO133" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="134" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>25</v>
       </c>
@@ -17445,8 +17844,11 @@
       <c r="AN134">
         <v>5.0550742099999999</v>
       </c>
+      <c r="AO134" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="135" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>230</v>
       </c>
@@ -17567,8 +17969,11 @@
       <c r="AN135">
         <v>2.1352081300000001</v>
       </c>
+      <c r="AO135" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="136" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>71</v>
       </c>
@@ -17689,8 +18094,11 @@
       <c r="AN136">
         <v>1.7305823600000001</v>
       </c>
+      <c r="AO136" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="137" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>33</v>
       </c>
@@ -17811,8 +18219,11 @@
       <c r="AN137">
         <v>0.71048533999999997</v>
       </c>
+      <c r="AO137" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="138" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>216</v>
       </c>
@@ -17933,8 +18344,11 @@
       <c r="AN138">
         <v>3.6620504899999999</v>
       </c>
+      <c r="AO138" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="139" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>12</v>
       </c>
@@ -18055,8 +18469,11 @@
       <c r="AN139">
         <v>7.927073</v>
       </c>
+      <c r="AO139" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="140" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>17</v>
       </c>
@@ -18177,8 +18594,11 @@
       <c r="AN140">
         <v>1.4629916000000001</v>
       </c>
+      <c r="AO140" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="141" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>5</v>
       </c>
@@ -18299,8 +18719,11 @@
       <c r="AN141">
         <v>6.4751372299999996</v>
       </c>
+      <c r="AO141" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="142" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>54</v>
       </c>
@@ -18421,8 +18844,11 @@
       <c r="AN142" t="s">
         <v>154</v>
       </c>
+      <c r="AO142" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="143" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>57</v>
       </c>
@@ -18543,8 +18969,11 @@
       <c r="AN143">
         <v>6.8922028500000003</v>
       </c>
+      <c r="AO143" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="144" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>170</v>
       </c>
@@ -18665,8 +19094,11 @@
       <c r="AN144">
         <v>5.1227693600000004</v>
       </c>
+      <c r="AO144" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="145" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>219</v>
       </c>
@@ -18787,8 +19219,11 @@
       <c r="AN145">
         <v>2.4348328100000001</v>
       </c>
+      <c r="AO145" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="146" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>74</v>
       </c>
@@ -18909,8 +19344,11 @@
       <c r="AN146">
         <v>0.57829392000000002</v>
       </c>
+      <c r="AO146" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="147" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>23</v>
       </c>
@@ -19031,8 +19469,11 @@
       <c r="AN147" t="s">
         <v>154</v>
       </c>
+      <c r="AO147" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="148" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>117</v>
       </c>
@@ -19153,8 +19594,11 @@
       <c r="AN148">
         <v>8.5744552600000006</v>
       </c>
+      <c r="AO148" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="149" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>142</v>
       </c>
@@ -19275,8 +19719,11 @@
       <c r="AN149">
         <v>3.62180948</v>
       </c>
+      <c r="AO149" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="150" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>233</v>
       </c>
@@ -19397,8 +19844,11 @@
       <c r="AN150">
         <v>1.1378284700000001</v>
       </c>
+      <c r="AO150" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="151" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>145</v>
       </c>
@@ -19519,8 +19969,11 @@
       <c r="AN151">
         <v>6.4016356500000002</v>
       </c>
+      <c r="AO151" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="152" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>60</v>
       </c>
@@ -19641,8 +20094,11 @@
       <c r="AN152">
         <v>4.64304161</v>
       </c>
+      <c r="AO152" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="153" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>199</v>
       </c>
@@ -19763,8 +20219,11 @@
       <c r="AN153">
         <v>1.65798402</v>
       </c>
+      <c r="AO153" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="154" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>70</v>
       </c>
@@ -19885,8 +20344,11 @@
       <c r="AN154">
         <v>2.9119231700000001</v>
       </c>
+      <c r="AO154" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="155" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>28</v>
       </c>
@@ -20007,8 +20469,11 @@
       <c r="AN155">
         <v>3.2797732399999999</v>
       </c>
+      <c r="AO155" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="156" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>174</v>
       </c>
@@ -20129,8 +20594,11 @@
       <c r="AN156">
         <v>1.43694162</v>
       </c>
+      <c r="AO156" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="157" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>166</v>
       </c>
@@ -20251,8 +20719,11 @@
       <c r="AN157">
         <v>4.5003747900000004</v>
       </c>
+      <c r="AO157" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="158" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>49</v>
       </c>
@@ -20373,8 +20844,11 @@
       <c r="AN158">
         <v>5.7812461900000001</v>
       </c>
+      <c r="AO158" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="159" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>59</v>
       </c>
@@ -20495,8 +20969,11 @@
       <c r="AN159" t="s">
         <v>154</v>
       </c>
+      <c r="AO159" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="160" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>149</v>
       </c>
@@ -20617,8 +21094,11 @@
       <c r="AN160">
         <v>1.86285079</v>
       </c>
+      <c r="AO160" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="161" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -20739,8 +21219,11 @@
       <c r="AN161">
         <v>4.4280986799999997</v>
       </c>
+      <c r="AO161" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="162" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>4</v>
       </c>
@@ -20861,8 +21344,11 @@
       <c r="AN162">
         <v>3.1606526399999999</v>
       </c>
+      <c r="AO162" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="163" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>157</v>
       </c>
@@ -20983,8 +21469,11 @@
       <c r="AN163">
         <v>2.3743403000000001</v>
       </c>
+      <c r="AO163" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="164" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>195</v>
       </c>
@@ -21105,8 +21594,11 @@
       <c r="AN164">
         <v>3.76377249</v>
       </c>
+      <c r="AO164" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="165" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>87</v>
       </c>
@@ -21227,8 +21719,11 @@
       <c r="AN165">
         <v>5.9962401400000003</v>
       </c>
+      <c r="AO165" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="166" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>172</v>
       </c>
@@ -21349,8 +21844,11 @@
       <c r="AN166">
         <v>2.7548310800000002</v>
       </c>
+      <c r="AO166" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="167" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>192</v>
       </c>
@@ -21471,8 +21969,11 @@
       <c r="AN167">
         <v>3.9720170499999998</v>
       </c>
+      <c r="AO167" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="168" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>111</v>
       </c>
@@ -21593,8 +22094,11 @@
       <c r="AN168">
         <v>0.94568121000000005</v>
       </c>
+      <c r="AO168" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="169" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>239</v>
       </c>
@@ -21715,8 +22219,11 @@
       <c r="AN169">
         <v>5.0694293999999998</v>
       </c>
+      <c r="AO169" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="170" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>138</v>
       </c>
@@ -21837,8 +22344,11 @@
       <c r="AN170">
         <v>3.80567455</v>
       </c>
+      <c r="AO170" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="171" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>75</v>
       </c>
@@ -21959,8 +22469,11 @@
       <c r="AN171">
         <v>1.56026566</v>
       </c>
+      <c r="AO171" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="172" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>66</v>
       </c>
@@ -22081,8 +22594,11 @@
       <c r="AN172">
         <v>2.2476420400000001</v>
       </c>
+      <c r="AO172" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="173" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>6</v>
       </c>
@@ -22203,8 +22719,11 @@
       <c r="AN173" t="s">
         <v>154</v>
       </c>
+      <c r="AO173" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="174" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>51</v>
       </c>
@@ -22325,8 +22844,11 @@
       <c r="AN174">
         <v>5.2982392300000001</v>
       </c>
+      <c r="AO174" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="175" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>11</v>
       </c>
@@ -22447,8 +22969,11 @@
       <c r="AN175">
         <v>6.0091485999999996</v>
       </c>
+      <c r="AO175" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="176" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>158</v>
       </c>
@@ -22569,8 +23094,11 @@
       <c r="AN176">
         <v>3.5372927199999999</v>
       </c>
+      <c r="AO176" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="177" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>50</v>
       </c>
@@ -22691,8 +23219,11 @@
       <c r="AN177" t="s">
         <v>154</v>
       </c>
+      <c r="AO177" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="178" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>48</v>
       </c>
@@ -22813,8 +23344,11 @@
       <c r="AN178">
         <v>4.4609417899999997</v>
       </c>
+      <c r="AO178" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="179" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>35</v>
       </c>
@@ -22935,8 +23469,11 @@
       <c r="AN179">
         <v>0.68977403999999998</v>
       </c>
+      <c r="AO179" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="180" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>176</v>
       </c>
@@ -23057,8 +23594,11 @@
       <c r="AN180">
         <v>6.3203930899999996</v>
       </c>
+      <c r="AO180" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="181" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>64</v>
       </c>
@@ -23179,8 +23719,11 @@
       <c r="AN181">
         <v>1.54440343</v>
       </c>
+      <c r="AO181" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="182" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>190</v>
       </c>
@@ -23301,8 +23844,11 @@
       <c r="AN182">
         <v>2.4708540399999999</v>
       </c>
+      <c r="AO182" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="183" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>0</v>
       </c>
@@ -23423,8 +23969,11 @@
       <c r="AN183">
         <v>2.0782704399999998</v>
       </c>
+      <c r="AO183" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="184" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>240</v>
       </c>
@@ -23545,8 +24094,11 @@
       <c r="AN184" t="s">
         <v>154</v>
       </c>
+      <c r="AO184" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="185" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>188</v>
       </c>
@@ -23667,8 +24219,11 @@
       <c r="AN185">
         <v>3.0514159200000002</v>
       </c>
+      <c r="AO185" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="186" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>44</v>
       </c>
@@ -23789,8 +24344,11 @@
       <c r="AN186">
         <v>1.0309916699999999</v>
       </c>
+      <c r="AO186" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="187" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>184</v>
       </c>
@@ -23911,8 +24469,11 @@
       <c r="AN187">
         <v>5.2543420799999998</v>
       </c>
+      <c r="AO187" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="188" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>153</v>
       </c>
@@ -24033,8 +24594,11 @@
       <c r="AN188">
         <v>2.1498565699999999</v>
       </c>
+      <c r="AO188" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="189" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>197</v>
       </c>
@@ -24155,8 +24719,11 @@
       <c r="AN189">
         <v>9.2737703299999996</v>
       </c>
+      <c r="AO189" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="190" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>27</v>
       </c>
@@ -24277,8 +24844,11 @@
       <c r="AN190">
         <v>3.70784402</v>
       </c>
+      <c r="AO190" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="191" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>99</v>
       </c>
@@ -24399,8 +24969,11 @@
       <c r="AN191" t="s">
         <v>154</v>
       </c>
+      <c r="AO191" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="192" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>76</v>
       </c>
@@ -24521,8 +25094,11 @@
       <c r="AN192">
         <v>1.9579576299999999</v>
       </c>
+      <c r="AO192" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="193" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>91</v>
       </c>
@@ -24643,8 +25219,11 @@
       <c r="AN193">
         <v>1.55844319</v>
       </c>
+      <c r="AO193" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="194" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>237</v>
       </c>
@@ -24765,8 +25344,11 @@
       <c r="AN194">
         <v>2.8930504300000002</v>
       </c>
+      <c r="AO194" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="195" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>15</v>
       </c>
@@ -24887,8 +25469,11 @@
       <c r="AN195">
         <v>2.62370276</v>
       </c>
+      <c r="AO195" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="196" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>61</v>
       </c>
@@ -25009,8 +25594,11 @@
       <c r="AN196">
         <v>1.05069971</v>
       </c>
+      <c r="AO196" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="197" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>205</v>
       </c>
@@ -25131,8 +25719,11 @@
       <c r="AN197">
         <v>3.2233376499999999</v>
       </c>
+      <c r="AO197" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="198" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>214</v>
       </c>
@@ -25253,8 +25844,11 @@
       <c r="AN198">
         <v>3.4165163000000001</v>
       </c>
+      <c r="AO198" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="199" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>242</v>
       </c>
@@ -25375,8 +25969,11 @@
       <c r="AN199">
         <v>4.1833572400000003</v>
       </c>
+      <c r="AO199" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="200" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>201</v>
       </c>
@@ -25497,8 +26094,11 @@
       <c r="AN200">
         <v>3.1913537999999999</v>
       </c>
+      <c r="AO200" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="201" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>185</v>
       </c>
@@ -25619,8 +26219,11 @@
       <c r="AN201">
         <v>1.19694495</v>
       </c>
+      <c r="AO201" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="202" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>232</v>
       </c>
@@ -25741,8 +26344,11 @@
       <c r="AN202" t="s">
         <v>154</v>
       </c>
+      <c r="AO202" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="203" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>52</v>
       </c>
@@ -25863,8 +26469,11 @@
       <c r="AN203">
         <v>15.21263409</v>
       </c>
+      <c r="AO203" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="204" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>119</v>
       </c>
@@ -25985,8 +26594,11 @@
       <c r="AN204">
         <v>1.0331534099999999</v>
       </c>
+      <c r="AO204" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="205" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>79</v>
       </c>
@@ -26107,8 +26719,11 @@
       <c r="AN205">
         <v>3.7030708799999998</v>
       </c>
+      <c r="AO205" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="206" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>22</v>
       </c>
@@ -26229,8 +26844,11 @@
       <c r="AN206">
         <v>2.1796560299999999</v>
       </c>
+      <c r="AO206" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="207" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>124</v>
       </c>
@@ -26351,8 +26969,11 @@
       <c r="AN207">
         <v>7.8579835899999999</v>
       </c>
+      <c r="AO207" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="208" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>130</v>
       </c>
@@ -26473,8 +27094,11 @@
       <c r="AN208">
         <v>8.5123634300000006</v>
       </c>
+      <c r="AO208" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="209" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>82</v>
       </c>
@@ -26595,8 +27219,11 @@
       <c r="AN209">
         <v>6.7149257699999998</v>
       </c>
+      <c r="AO209" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="210" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>103</v>
       </c>
@@ -26717,8 +27344,11 @@
       <c r="AN210">
         <v>2.0197141200000002</v>
       </c>
+      <c r="AO210" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="211" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>210</v>
       </c>
@@ -26839,8 +27469,11 @@
       <c r="AN211">
         <v>2.1413815</v>
       </c>
+      <c r="AO211" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="212" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>156</v>
       </c>
@@ -26961,8 +27594,11 @@
       <c r="AN212">
         <v>1.7046546899999999</v>
       </c>
+      <c r="AO212" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="213" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>132</v>
       </c>
@@ -27083,8 +27719,11 @@
       <c r="AN213">
         <v>2.6962101500000002</v>
       </c>
+      <c r="AO213" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="214" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>26</v>
       </c>
@@ -27205,8 +27844,11 @@
       <c r="AN214" t="s">
         <v>154</v>
       </c>
+      <c r="AO214" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="215" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>40</v>
       </c>
@@ -27327,8 +27969,11 @@
       <c r="AN215" t="s">
         <v>154</v>
       </c>
+      <c r="AO215" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="216" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>39</v>
       </c>
@@ -27449,8 +28094,11 @@
       <c r="AN216" t="s">
         <v>154</v>
       </c>
+      <c r="AO216" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="217" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>159</v>
       </c>
@@ -27571,8 +28219,11 @@
       <c r="AN217">
         <v>1.92871916</v>
       </c>
+      <c r="AO217" t="s">
+        <v>154</v>
+      </c>
     </row>
-    <row r="218" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>19</v>
       </c>
@@ -27692,6 +28343,9 @@
       </c>
       <c r="AN218">
         <v>1.3242476000000001</v>
+      </c>
+      <c r="AO218" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>